<commit_message>
se agrego un for
</commit_message>
<xml_diff>
--- a/testdata/coppel-data.xlsx
+++ b/testdata/coppel-data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -678,10 +678,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -796,6 +796,54 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>Si</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MCP-INT-01</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://www.coppel.com/</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Julian</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Medina</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>6672108838</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>HolaMundo</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -816,7 +864,7 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
agregando resgistros al excel
</commit_message>
<xml_diff>
--- a/testdata/coppel-data.xlsx
+++ b/testdata/coppel-data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -68,13 +68,17 @@
       <protection locked="0" hidden="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment vertical="top"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,10 +682,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -833,8 +837,10 @@
           <t>Masculino</t>
         </is>
       </c>
-      <c r="H3" t="n">
-        <v>6672108838</v>
+      <c r="H3" s="4" t="inlineStr">
+        <is>
+          <t>hrpinam@gmail.com</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -844,12 +850,20 @@
       <c r="J3" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>S</t>
         </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -862,10 +876,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -980,6 +994,54 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MCP-INT-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://www.coppel.com/</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Femenino</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>6672529402</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>contra123contra</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Si</t>
         </is>
       </c>
     </row>

</xml_diff>